<commit_message>
rajout ajustement de la largeur des colonnes
</commit_message>
<xml_diff>
--- a/test/resultat reportsb.xlsx
+++ b/test/resultat reportsb.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpeti\Desktop\swiiborg\Swissborg-reporting\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0801AE54-C7C2-4EBA-AD23-B6C7EE99A10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="326" yWindow="377" windowWidth="24360" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="EUR" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="BTC" sheetId="3" r:id="rId3"/>
     <sheet name="DOT" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -31,13 +25,13 @@
     <t>Compte</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Operation</t>
   </si>
   <si>
     <t>Montant euro</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>cours</t>
@@ -127,11 +121,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d\ mmm\ yyyy\ \ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="d mmm yyyy  hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,21 +189,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +233,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -281,7 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -316,10 +301,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -492,67 +476,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="13.61328125" customWidth="1"/>
-    <col min="6" max="6" width="20.61328125" customWidth="1"/>
-    <col min="7" max="9" width="13.61328125" customWidth="1"/>
-    <col min="10" max="10" width="17.4609375" customWidth="1"/>
-    <col min="11" max="11" width="19.3828125" customWidth="1"/>
-    <col min="12" max="12" width="13.61328125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="91.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44671.33490740741</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -560,14 +552,14 @@
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="F2" s="2">
-        <v>44671.334907407407</v>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -575,19 +567,16 @@
       <c r="J2">
         <v>100</v>
       </c>
-      <c r="K2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44672.33035879629</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -595,14 +584,14 @@
       <c r="E3">
         <v>250</v>
       </c>
-      <c r="F3" s="2">
-        <v>44672.330358796287</v>
+      <c r="F3">
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="I3">
         <v>250</v>
@@ -610,19 +599,16 @@
       <c r="J3">
         <v>250</v>
       </c>
-      <c r="K3">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
-        <v>3</v>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44677.61417824074</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -630,37 +616,34 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="2">
-        <v>44677.614178240743</v>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="J4">
         <v>-100</v>
       </c>
-      <c r="K4">
-        <v>-100</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
-        <v>5</v>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44677.75449074074</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -668,37 +651,34 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
-        <v>44677.754490740743</v>
+      <c r="F5">
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-250</v>
       </c>
       <c r="J5">
         <v>-250</v>
       </c>
-      <c r="K5">
-        <v>-250</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
-        <v>7</v>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44678.32908564815</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -706,14 +686,14 @@
       <c r="E6">
         <v>400</v>
       </c>
-      <c r="F6" s="2">
-        <v>44678.329085648147</v>
+      <c r="F6">
+        <v>1</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="I6">
         <v>400</v>
@@ -721,19 +701,16 @@
       <c r="J6">
         <v>400</v>
       </c>
-      <c r="K6">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
-        <v>8</v>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -741,72 +718,66 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="2">
-        <v>44678.367939814823</v>
+      <c r="F7">
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>-5041.892681</v>
       </c>
       <c r="J7">
-        <v>-5041.8926810000003</v>
-      </c>
-      <c r="K7">
-        <v>-5041.8926810000003</v>
-      </c>
-      <c r="L7" t="s">
+        <v>-5041.892681</v>
+      </c>
+      <c r="K7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="1">
-        <v>15</v>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44683.43067129629</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8">
-        <v>151.57658000000001</v>
-      </c>
-      <c r="F8" s="2">
-        <v>44683.430671296293</v>
+        <v>151.57658</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>151.57658</v>
       </c>
       <c r="I8">
-        <v>151.57658000000001</v>
+        <v>151.57658</v>
       </c>
       <c r="J8">
-        <v>151.57658000000001</v>
-      </c>
-      <c r="K8">
-        <v>151.57658000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="1">
-        <v>17</v>
+        <v>151.57658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44684.74471064815</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -814,72 +785,66 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="2">
-        <v>44684.744710648149</v>
+      <c r="F9">
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>-301.57658</v>
       </c>
       <c r="J9">
-        <v>-301.57657999999998</v>
-      </c>
-      <c r="K9">
-        <v>-301.57657999999998</v>
-      </c>
-      <c r="L9" t="s">
+        <v>-301.57658</v>
+      </c>
+      <c r="K9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="1">
-        <v>19</v>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44685.3312962963</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="E10">
-        <v>451.57657999999998</v>
-      </c>
-      <c r="F10" s="2">
-        <v>44685.331296296303</v>
+        <v>451.57658</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>451.57658</v>
       </c>
       <c r="I10">
-        <v>451.57657999999998</v>
+        <v>451.57658</v>
       </c>
       <c r="J10">
-        <v>451.57657999999998</v>
-      </c>
-      <c r="K10">
-        <v>451.57657999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A11" s="1">
-        <v>20</v>
+        <v>451.57658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44685.33789351852</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -887,37 +852,34 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="2">
-        <v>44685.337893518517</v>
+      <c r="F11">
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>-163.9154266695899</v>
       </c>
       <c r="J11">
-        <v>-163.91542666958989</v>
-      </c>
-      <c r="K11">
-        <v>-163.91542666958989</v>
-      </c>
-      <c r="L11" t="s">
+        <v>-163.9154266695899</v>
+      </c>
+      <c r="K11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="1">
-        <v>23</v>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44685.48255787037</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -925,107 +887,98 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="2">
-        <v>44685.482557870368</v>
+      <c r="F12">
+        <v>1</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>-150.01375229347</v>
       </c>
       <c r="J12">
-        <v>-150.01375229346999</v>
-      </c>
-      <c r="K12">
-        <v>-150.01375229346999</v>
-      </c>
-      <c r="L12" t="s">
+        <v>-150.01375229347</v>
+      </c>
+      <c r="K12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A13" s="1">
-        <v>34</v>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44690.33619212963</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13">
-        <v>150.00256739220001</v>
-      </c>
-      <c r="F13" s="2">
-        <v>44690.336192129631</v>
+        <v>150.0025673922</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>150.0025673922</v>
       </c>
       <c r="I13">
-        <v>150.00256739220001</v>
+        <v>150.0025673922</v>
       </c>
       <c r="J13">
-        <v>150.00256739220001</v>
-      </c>
-      <c r="K13">
-        <v>150.00256739220001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="1">
-        <v>35</v>
+        <v>150.0025673922</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44690.33686342592</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14">
-        <v>152.22108399999999</v>
-      </c>
-      <c r="F14" s="2">
-        <v>44690.336863425917</v>
+        <v>152.221084</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>152.221084</v>
       </c>
       <c r="I14">
-        <v>152.22108399999999</v>
+        <v>152.221084</v>
       </c>
       <c r="J14">
-        <v>152.22108399999999</v>
-      </c>
-      <c r="K14">
-        <v>152.22108399999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A15" s="1">
-        <v>36</v>
+        <v>152.221084</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44690.3628125</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -1033,37 +986,34 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="2">
-        <v>44690.362812500003</v>
+      <c r="F15">
+        <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>-300.0025673922</v>
       </c>
       <c r="J15">
-        <v>-300.00256739219998</v>
-      </c>
-      <c r="K15">
-        <v>-300.00256739219998</v>
-      </c>
-      <c r="L15" t="s">
+        <v>-300.0025673922</v>
+      </c>
+      <c r="K15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" s="1">
-        <v>39</v>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44690.4465162037</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1071,37 +1021,34 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="2">
-        <v>44690.446516203701</v>
+      <c r="F16">
+        <v>1</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>-150.0025678104</v>
       </c>
       <c r="J16">
         <v>-150.0025678104</v>
       </c>
-      <c r="K16">
-        <v>-150.0025678104</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="K16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" s="1">
-        <v>40</v>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44690.60130787037</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -1109,37 +1056,34 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
-        <v>44690.601307870369</v>
+      <c r="F17">
+        <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>-300.0025678104</v>
       </c>
       <c r="J17">
-        <v>-300.00256781040002</v>
-      </c>
-      <c r="K17">
-        <v>-300.00256781040002</v>
-      </c>
-      <c r="L17" t="s">
+        <v>-300.0025678104</v>
+      </c>
+      <c r="K17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A18" s="1">
-        <v>41</v>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44690.8674537037</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -1147,37 +1091,34 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" s="2">
-        <v>44690.8674537037</v>
+      <c r="F18">
+        <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>-450.0025678104</v>
       </c>
       <c r="J18">
-        <v>-450.00256781040002</v>
-      </c>
-      <c r="K18">
-        <v>-450.00256781040002</v>
-      </c>
-      <c r="L18" t="s">
+        <v>-450.0025678104</v>
+      </c>
+      <c r="K18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A19" s="1">
-        <v>42</v>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44691.00876157408</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1185,72 +1126,66 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" s="2">
-        <v>44691.008761574078</v>
+      <c r="F19">
+        <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>-600.0025678104</v>
       </c>
       <c r="J19">
-        <v>-600.00256781040002</v>
-      </c>
-      <c r="K19">
-        <v>-600.00256781040002</v>
-      </c>
-      <c r="L19" t="s">
+        <v>-600.0025678104</v>
+      </c>
+      <c r="K19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A20" s="1">
-        <v>43</v>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44691.33443287037</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="E20">
-        <v>750.00256781040002</v>
-      </c>
-      <c r="F20" s="2">
-        <v>44691.334432870368</v>
+        <v>750.0025678104</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>750.0025678104</v>
       </c>
       <c r="I20">
-        <v>750.00256781040002</v>
+        <v>750.0025678104</v>
       </c>
       <c r="J20">
-        <v>750.00256781040002</v>
-      </c>
-      <c r="K20">
-        <v>750.00256781040002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A21" s="1">
-        <v>46</v>
+        <v>750.0025678104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44691.45037037037</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -1258,37 +1193,34 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21" s="2">
-        <v>44691.450370370367</v>
+      <c r="F21">
+        <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>-150.0016707659</v>
       </c>
       <c r="J21">
         <v>-150.0016707659</v>
       </c>
-      <c r="K21">
-        <v>-150.0016707659</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="K21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A22" s="1">
-        <v>47</v>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44691.71796296296</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -1296,37 +1228,34 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" s="2">
-        <v>44691.717962962961</v>
+      <c r="F22">
+        <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>-300.0016707659</v>
       </c>
       <c r="J22">
-        <v>-300.00167076589997</v>
-      </c>
-      <c r="K22">
-        <v>-300.00167076589997</v>
-      </c>
-      <c r="L22" t="s">
+        <v>-300.0016707659</v>
+      </c>
+      <c r="K22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A23" s="1">
-        <v>48</v>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44691.99467592593</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -1334,72 +1263,66 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="2">
-        <v>44691.994675925933</v>
+      <c r="F23">
+        <v>1</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>-450.0016707659</v>
       </c>
       <c r="J23">
-        <v>-450.00167076589997</v>
-      </c>
-      <c r="K23">
-        <v>-450.00167076589997</v>
-      </c>
-      <c r="L23" t="s">
+        <v>-450.0016707659</v>
+      </c>
+      <c r="K23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A24" s="1">
-        <v>49</v>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44692.3317824074</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="E24">
-        <v>600.00167076590003</v>
-      </c>
-      <c r="F24" s="2">
-        <v>44692.331782407397</v>
+        <v>600.0016707659</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>600.0016707659</v>
       </c>
       <c r="I24">
-        <v>600.00167076590003</v>
+        <v>600.0016707659</v>
       </c>
       <c r="J24">
-        <v>600.00167076590003</v>
-      </c>
-      <c r="K24">
-        <v>600.00167076590003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A25" s="1">
-        <v>52</v>
+        <v>600.0016707659</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44692.62164351852</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1407,37 +1330,34 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="2">
-        <v>44692.62164351852</v>
+      <c r="F25">
+        <v>1</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>-150.0016709427</v>
       </c>
       <c r="J25">
         <v>-150.0016709427</v>
       </c>
-      <c r="K25">
-        <v>-150.0016709427</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="K25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A26" s="1">
-        <v>53</v>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44692.8556712963</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -1445,37 +1365,34 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="2">
-        <v>44692.855671296304</v>
+      <c r="F26">
+        <v>1</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>-300.0016709427</v>
       </c>
       <c r="J26">
         <v>-300.0016709427</v>
       </c>
-      <c r="K26">
-        <v>-300.0016709427</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="K26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A27" s="1">
-        <v>54</v>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44692.89680555555</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -1483,37 +1400,34 @@
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" s="2">
-        <v>44692.896805555552</v>
+      <c r="F27">
+        <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>-450.0016709427</v>
       </c>
       <c r="J27">
         <v>-450.0016709427</v>
       </c>
-      <c r="K27">
-        <v>-450.0016709427</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="K27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A28" s="1">
-        <v>56</v>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44692.90526620371</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -1521,37 +1435,34 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="2">
-        <v>44692.905266203707</v>
+      <c r="F28">
+        <v>1</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>-600.0016709427</v>
       </c>
       <c r="J28">
         <v>-600.0016709427</v>
       </c>
-      <c r="K28">
-        <v>-600.0016709427</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="K28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A29" s="1">
-        <v>58</v>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44692.93699074074</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
@@ -1559,37 +1470,34 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="2">
-        <v>44692.936990740738</v>
+      <c r="F29">
+        <v>1</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>-750.0016709427</v>
       </c>
       <c r="J29">
         <v>-750.0016709427</v>
       </c>
-      <c r="K29">
-        <v>-750.0016709427</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="K29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A30" s="1">
-        <v>63</v>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44693.45594907407</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1597,14 +1505,14 @@
       <c r="E30">
         <v>150.0016711195</v>
       </c>
-      <c r="F30" s="2">
-        <v>44693.455949074072</v>
+      <c r="F30">
+        <v>1</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>150.0016711195</v>
       </c>
       <c r="I30">
         <v>150.0016711195</v>
@@ -1612,89 +1520,80 @@
       <c r="J30">
         <v>150.0016711195</v>
       </c>
-      <c r="K30">
-        <v>150.0016711195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A31" s="1">
-        <v>64</v>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C31" s="2">
+        <v>44693.45594907407</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
       </c>
       <c r="E31">
-        <v>152.58619999999999</v>
-      </c>
-      <c r="F31" s="2">
-        <v>44693.455949074072</v>
+        <v>152.5862</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>152.5862</v>
       </c>
       <c r="I31">
-        <v>152.58619999999999</v>
+        <v>152.5862</v>
       </c>
       <c r="J31">
-        <v>152.58619999999999</v>
-      </c>
-      <c r="K31">
-        <v>152.58619999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A32" s="1">
-        <v>65</v>
+        <v>152.5862</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44693.45594907407</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32">
-        <v>300.00167111949997</v>
-      </c>
-      <c r="F32" s="2">
-        <v>44693.455949074072</v>
+        <v>300.0016711195</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>300.0016711195</v>
       </c>
       <c r="I32">
-        <v>300.00167111949997</v>
+        <v>300.0016711195</v>
       </c>
       <c r="J32">
-        <v>300.00167111949997</v>
-      </c>
-      <c r="K32">
-        <v>300.00167111949997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A33" s="1">
-        <v>66</v>
+        <v>300.0016711195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C33" s="2">
+        <v>44693.45594907407</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -1702,14 +1601,14 @@
       <c r="E33">
         <v>12345</v>
       </c>
-      <c r="F33" s="2">
-        <v>44693.455949074072</v>
+      <c r="F33">
+        <v>1</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>12345</v>
       </c>
       <c r="I33">
         <v>12345</v>
@@ -1717,19 +1616,16 @@
       <c r="J33">
         <v>12345</v>
       </c>
-      <c r="K33">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A34" s="1">
-        <v>78</v>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C34" s="2">
+        <v>44695.64142361111</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
@@ -1737,37 +1633,34 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34" s="2">
-        <v>44695.641423611109</v>
+      <c r="F34">
+        <v>1</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>-150.0043046123</v>
       </c>
       <c r="J34">
-        <v>-150.00430461229999</v>
-      </c>
-      <c r="K34">
-        <v>-150.00430461229999</v>
-      </c>
-      <c r="L34" t="s">
+        <v>-150.0043046123</v>
+      </c>
+      <c r="K34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A35" s="1">
-        <v>79</v>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44695.73297453704</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
@@ -1775,37 +1668,34 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" s="2">
-        <v>44695.732974537037</v>
+      <c r="F35">
+        <v>1</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>-300.0043046123</v>
       </c>
       <c r="J35">
-        <v>-300.00430461230002</v>
-      </c>
-      <c r="K35">
-        <v>-300.00430461230002</v>
-      </c>
-      <c r="L35" t="s">
+        <v>-300.0043046123</v>
+      </c>
+      <c r="K35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A36" s="1">
-        <v>82</v>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44696.5969675926</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -1813,37 +1703,34 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36" s="2">
-        <v>44696.596967592603</v>
+      <c r="F36">
+        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>-150.0043057899</v>
       </c>
       <c r="J36">
         <v>-150.0043057899</v>
       </c>
-      <c r="K36">
-        <v>-150.0043057899</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="K36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A37" s="1">
-        <v>84</v>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44696.67313657407</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
@@ -1851,37 +1738,34 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37" s="2">
-        <v>44696.673136574071</v>
+      <c r="F37">
+        <v>1</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>-300.0043057899</v>
       </c>
       <c r="J37">
         <v>-300.0043057899</v>
       </c>
-      <c r="K37">
-        <v>-300.0043057899</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="K37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A38" s="1">
-        <v>86</v>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C38" s="2">
+        <v>44696.69998842593</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
@@ -1889,25 +1773,22 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38" s="2">
-        <v>44696.699988425928</v>
+      <c r="F38">
+        <v>1</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>-450.0043057899</v>
       </c>
       <c r="J38">
         <v>-450.0043057899</v>
       </c>
-      <c r="K38">
-        <v>-450.0043057899</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="K38" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1917,62 +1798,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1048576"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="12" width="18.61328125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>4</v>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44677.61417824074</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -1980,34 +1874,31 @@
       <c r="E2">
         <v>2023.2</v>
       </c>
-      <c r="F2" s="2">
-        <v>44677.614178240743</v>
+      <c r="F2">
+        <v>0.400594</v>
       </c>
       <c r="G2">
-        <v>0.40059400000000001</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2023.2</v>
       </c>
       <c r="I2">
-        <v>2023.2</v>
+        <v>5000</v>
       </c>
       <c r="J2">
         <v>5000</v>
       </c>
-      <c r="K2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
-        <v>6</v>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44677.75449074074</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -2015,81 +1906,72 @@
       <c r="E3">
         <v>1900</v>
       </c>
-      <c r="F3" s="2">
-        <v>44677.754490740743</v>
+      <c r="F3">
+        <v>0.3883977274030472</v>
       </c>
       <c r="G3">
-        <v>0.38839772740304718</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>1900</v>
       </c>
       <c r="I3">
-        <v>1900</v>
+        <v>4867.433217595</v>
       </c>
       <c r="J3">
-        <v>4867.4332175950003</v>
-      </c>
-      <c r="K3">
-        <v>4867.4332175950003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
-        <v>24</v>
+        <v>4867.433217595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44685.48255787037</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4">
-        <v>1865.5052968227001</v>
-      </c>
-      <c r="F4" s="2">
-        <v>44685.482557870368</v>
+        <v>1865.5052968227</v>
+      </c>
+      <c r="F4">
+        <v>0.3632441820595023</v>
       </c>
       <c r="G4">
-        <v>0.36324418205950232</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>1865.5052968227</v>
       </c>
       <c r="I4">
-        <v>1865.5052968227001</v>
+        <v>5110</v>
       </c>
       <c r="J4">
         <v>5110</v>
       </c>
-      <c r="K4">
-        <v>5110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
-        <v>88</v>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="H5">
-        <v>1</v>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>50.45521599999999</v>
       </c>
       <c r="J5">
-        <v>50.455215999999993</v>
-      </c>
-      <c r="K5">
-        <v>50.455215999999993</v>
+        <v>50.45521599999999</v>
       </c>
     </row>
   </sheetData>
@@ -2098,62 +1980,75 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="12" width="17.4609375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>9</v>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -2161,34 +2056,31 @@
       <c r="E2">
         <v>1500</v>
       </c>
-      <c r="F2" s="2">
-        <v>44678.367939814823</v>
+      <c r="F2">
+        <v>36370.2893825163</v>
       </c>
       <c r="G2">
-        <v>36370.289382516297</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>1500</v>
       </c>
       <c r="I2">
-        <v>1500</v>
+        <v>0.04103624209043179</v>
       </c>
       <c r="J2">
-        <v>4.1036242090431788E-2</v>
-      </c>
-      <c r="K2">
-        <v>4.1036242090431788E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
-        <v>21</v>
+        <v>0.04103624209043179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -2196,34 +2088,31 @@
       <c r="E3">
         <v>500</v>
       </c>
-      <c r="F3" s="2">
-        <v>44678.367939814823</v>
+      <c r="F3">
+        <v>36357.57199999997</v>
       </c>
       <c r="G3">
-        <v>36357.571999999971</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I3">
-        <v>500</v>
+        <v>0.01368353200263209</v>
       </c>
       <c r="J3">
-        <v>1.3683532002632091E-2</v>
-      </c>
-      <c r="K3">
-        <v>1.3683532002632091E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
-        <v>26</v>
+        <v>0.01368353200263209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -2231,34 +2120,31 @@
       <c r="E4">
         <v>1500</v>
       </c>
-      <c r="F4" s="2">
-        <v>44678.367939814823</v>
+      <c r="F4">
+        <v>35330.01649366671</v>
       </c>
       <c r="G4">
-        <v>35330.016493666713</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>1500</v>
       </c>
       <c r="I4">
-        <v>1500</v>
+        <v>0.04224453165108334</v>
       </c>
       <c r="J4">
-        <v>4.2244531651083342E-2</v>
-      </c>
-      <c r="K4">
-        <v>4.2244531651083342E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
-        <v>27</v>
+        <v>0.04224453165108334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -2266,34 +2152,31 @@
       <c r="E5">
         <v>1500</v>
       </c>
-      <c r="F5" s="2">
-        <v>44678.367939814823</v>
+      <c r="F5">
+        <v>35220.05380000041</v>
       </c>
       <c r="G5">
-        <v>35220.053800000409</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>1500</v>
       </c>
       <c r="I5">
-        <v>1500</v>
+        <v>0.042376425898588</v>
       </c>
       <c r="J5">
-        <v>4.2376425898587998E-2</v>
-      </c>
-      <c r="K5">
-        <v>4.2376425898587998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
-        <v>55</v>
+        <v>0.042376425898588</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -2301,34 +2184,31 @@
       <c r="E6">
         <v>1000</v>
       </c>
-      <c r="F6" s="2">
-        <v>44678.367939814823</v>
+      <c r="F6">
+        <v>28164.39185381187</v>
       </c>
       <c r="G6">
-        <v>28164.391853811871</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I6">
-        <v>1000</v>
+        <v>0.03532829699162608</v>
       </c>
       <c r="J6">
-        <v>3.5328296991626082E-2</v>
-      </c>
-      <c r="K6">
-        <v>3.5328296991626082E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
-        <v>57</v>
+        <v>0.03532829699162608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -2336,34 +2216,31 @@
       <c r="E7">
         <v>1000</v>
       </c>
-      <c r="F7" s="2">
-        <v>44678.367939814823</v>
+      <c r="F7">
+        <v>27833.99375000024</v>
       </c>
       <c r="G7">
-        <v>27833.993750000242</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I7">
-        <v>1000</v>
+        <v>0.03574765478992721</v>
       </c>
       <c r="J7">
-        <v>3.5747654789927211E-2</v>
-      </c>
-      <c r="K7">
-        <v>3.5747654789927211E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="1">
-        <v>59</v>
+        <v>0.03574765478992721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -2371,34 +2248,31 @@
       <c r="E8">
         <v>1000</v>
       </c>
-      <c r="F8" s="2">
-        <v>44678.367939814823</v>
+      <c r="F8">
+        <v>27743.41049999971</v>
       </c>
       <c r="G8">
-        <v>27743.410499999711</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I8">
-        <v>1000</v>
+        <v>0.03586437219029039</v>
       </c>
       <c r="J8">
-        <v>3.5864372190290393E-2</v>
-      </c>
-      <c r="K8">
-        <v>3.5864372190290393E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="1">
-        <v>60</v>
+        <v>0.03586437219029039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -2406,34 +2280,31 @@
       <c r="E9">
         <v>2500</v>
       </c>
-      <c r="F9" s="2">
-        <v>44678.367939814823</v>
+      <c r="F9">
+        <v>27210.28170000007</v>
       </c>
       <c r="G9">
-        <v>27210.281700000069</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>2500</v>
       </c>
       <c r="I9">
-        <v>2500</v>
+        <v>0.09141764967468137</v>
       </c>
       <c r="J9">
-        <v>9.141764967468137E-2</v>
-      </c>
-      <c r="K9">
-        <v>9.141764967468137E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="1">
-        <v>67</v>
+        <v>0.09141764967468137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -2441,34 +2312,31 @@
       <c r="E10">
         <v>1000</v>
       </c>
-      <c r="F10" s="2">
-        <v>44678.367939814823</v>
+      <c r="F10">
+        <v>26992.24225000007</v>
       </c>
       <c r="G10">
-        <v>26992.242250000068</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I10">
-        <v>1000</v>
+        <v>0.03686244331924657</v>
       </c>
       <c r="J10">
-        <v>3.6862443319246568E-2</v>
-      </c>
-      <c r="K10">
-        <v>3.6862443319246568E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A11" s="1">
-        <v>68</v>
+        <v>0.03686244331924657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -2476,34 +2344,31 @@
       <c r="E11">
         <v>1000</v>
       </c>
-      <c r="F11" s="2">
-        <v>44678.367939814823</v>
+      <c r="F11">
+        <v>27034.093289566</v>
       </c>
       <c r="G11">
-        <v>27034.093289566001</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I11">
-        <v>1000</v>
+        <v>0.03680537717105634</v>
       </c>
       <c r="J11">
-        <v>3.6805377171056343E-2</v>
-      </c>
-      <c r="K11">
-        <v>3.6805377171056343E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="1">
-        <v>69</v>
+        <v>0.03680537717105634</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
@@ -2511,34 +2376,31 @@
       <c r="E12">
         <v>1000</v>
       </c>
-      <c r="F12" s="2">
-        <v>44678.367939814823</v>
+      <c r="F12">
+        <v>28130.92875619538</v>
       </c>
       <c r="G12">
-        <v>28130.928756195379</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I12">
-        <v>1000</v>
+        <v>0.03537032170617074</v>
       </c>
       <c r="J12">
-        <v>3.5370321706170743E-2</v>
-      </c>
-      <c r="K12">
-        <v>3.5370321706170743E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A13" s="1">
-        <v>70</v>
+        <v>0.03537032170617074</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -2546,34 +2408,31 @@
       <c r="E13">
         <v>1000</v>
       </c>
-      <c r="F13" s="2">
-        <v>44678.367939814823</v>
+      <c r="F13">
+        <v>29351.48504985173</v>
       </c>
       <c r="G13">
-        <v>29351.48504985173</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I13">
-        <v>1000</v>
+        <v>0.03389947726018129</v>
       </c>
       <c r="J13">
-        <v>3.389947726018129E-2</v>
-      </c>
-      <c r="K13">
-        <v>3.389947726018129E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="1">
-        <v>73</v>
+        <v>0.03389947726018129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
@@ -2581,34 +2440,31 @@
       <c r="E14">
         <v>1000</v>
       </c>
-      <c r="F14" s="2">
-        <v>44678.367939814823</v>
+      <c r="F14">
+        <v>29221.03532755847</v>
       </c>
       <c r="G14">
-        <v>29221.035327558471</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I14">
-        <v>1000</v>
+        <v>0.03405081267129546</v>
       </c>
       <c r="J14">
-        <v>3.4050812671295463E-2</v>
-      </c>
-      <c r="K14">
-        <v>3.4050812671295463E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A15" s="1">
-        <v>74</v>
+        <v>0.03405081267129546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
@@ -2616,34 +2472,31 @@
       <c r="E15">
         <v>1000</v>
       </c>
-      <c r="F15" s="2">
-        <v>44678.367939814823</v>
+      <c r="F15">
+        <v>28784.91600000014</v>
       </c>
       <c r="G15">
-        <v>28784.916000000139</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I15">
-        <v>1000</v>
+        <v>0.03456671542831652</v>
       </c>
       <c r="J15">
-        <v>3.4566715428316519E-2</v>
-      </c>
-      <c r="K15">
-        <v>3.4566715428316519E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" s="1">
-        <v>75</v>
+        <v>0.03456671542831652</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D16" t="s">
         <v>27</v>
@@ -2651,34 +2504,31 @@
       <c r="E16">
         <v>1000</v>
       </c>
-      <c r="F16" s="2">
-        <v>44678.367939814823</v>
+      <c r="F16">
+        <v>28518.19413624944</v>
       </c>
       <c r="G16">
-        <v>28518.19413624944</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I16">
-        <v>1000</v>
+        <v>0.03489000724401608</v>
       </c>
       <c r="J16">
-        <v>3.4890007244016079E-2</v>
-      </c>
-      <c r="K16">
-        <v>3.4890007244016079E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="1">
-        <v>83</v>
+        <v>0.03489000724401608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D17" t="s">
         <v>27</v>
@@ -2686,34 +2536,31 @@
       <c r="E17">
         <v>500</v>
       </c>
-      <c r="F17" s="2">
-        <v>44678.367939814823</v>
+      <c r="F17">
+        <v>29230.77649999988</v>
       </c>
       <c r="G17">
-        <v>29230.77649999988</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I17">
-        <v>500</v>
+        <v>0.01701973260956657</v>
       </c>
       <c r="J17">
-        <v>1.701973260956657E-2</v>
-      </c>
-      <c r="K17">
-        <v>1.701973260956657E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="1">
-        <v>85</v>
+        <v>0.01701973260956657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D18" t="s">
         <v>27</v>
@@ -2721,58 +2568,52 @@
       <c r="E18">
         <v>1000</v>
       </c>
-      <c r="F18" s="2">
-        <v>44678.367939814823</v>
+      <c r="F18">
+        <v>28836.88849999984</v>
       </c>
       <c r="G18">
-        <v>28836.888499999841</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="I18">
-        <v>1000</v>
+        <v>0.03450441610578081</v>
       </c>
       <c r="J18">
-        <v>3.4504416105780811E-2</v>
-      </c>
-      <c r="K18">
-        <v>3.4504416105780811E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A19" s="1">
-        <v>87</v>
+        <v>0.03450441610578081</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44678.36793981482</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
       </c>
       <c r="E19">
-        <v>980.31420979999996</v>
-      </c>
-      <c r="F19" s="2">
-        <v>44678.367939814823</v>
+        <v>980.3142098</v>
+      </c>
+      <c r="F19">
+        <v>28827.07264055349</v>
       </c>
       <c r="G19">
-        <v>28827.072640553492</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>980.3142098</v>
       </c>
       <c r="I19">
-        <v>980.31420979999996</v>
+        <v>0.03383668716256691</v>
       </c>
       <c r="J19">
-        <v>3.3836687162566909E-2</v>
-      </c>
-      <c r="K19">
-        <v>3.3836687162566909E-2</v>
+        <v>0.03383668716256691</v>
       </c>
     </row>
   </sheetData>
@@ -2781,109 +2622,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="12" width="16.84375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>18</v>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44684.74471064815</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2">
-        <v>198.19085889999999</v>
-      </c>
-      <c r="F2" s="2">
-        <v>44684.744710648149</v>
+        <v>198.1908589</v>
+      </c>
+      <c r="F2">
+        <v>14.24252835402569</v>
       </c>
       <c r="G2">
-        <v>14.242528354025691</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>198.1908589</v>
       </c>
       <c r="I2">
-        <v>198.19085889999999</v>
+        <v>13.84584953624199</v>
       </c>
       <c r="J2">
-        <v>13.845849536241991</v>
-      </c>
-      <c r="K2">
-        <v>13.845849536241991</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
-        <v>88</v>
+        <v>13.84584953624199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.0235362896</v>
       </c>
       <c r="J3">
-        <v>2.35362896E-2</v>
-      </c>
-      <c r="K3">
-        <v>2.35362896E-2</v>
+        <v>0.0235362896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>